<commit_message>
Minor tweak to ESPN NFL section
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data.xlsx
+++ b/com.espn/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zainj\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DA89EF-1238-4A00-940D-3C2E7F60B1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDD99E5-8B2E-40FC-A02B-7A2D6DC00663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{723F212A-670C-4A3B-B8E6-389E6F040CFB}"/>
   </bookViews>
@@ -32,6 +32,110 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>Buffalo Bills</t>
+  </si>
+  <si>
+    <t>Miami Dolphins</t>
+  </si>
+  <si>
+    <t>New England Patriots</t>
+  </si>
+  <si>
+    <t>New York Jets</t>
+  </si>
+  <si>
+    <t>Baltimore Ravens</t>
+  </si>
+  <si>
+    <t>Cincinnati Bengals</t>
+  </si>
+  <si>
+    <t>Cleveland Browns</t>
+  </si>
+  <si>
+    <t>Pittsburgh Steelers</t>
+  </si>
+  <si>
+    <t>Houston Texans</t>
+  </si>
+  <si>
+    <t>Jacksonville Jaguars</t>
+  </si>
+  <si>
+    <t>Denver Broncos</t>
+  </si>
+  <si>
+    <t>Kansas City Chiefs</t>
+  </si>
+  <si>
+    <t>Las Vegas Raiders</t>
+  </si>
+  <si>
+    <t>Los Angeles Chargers</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys</t>
+  </si>
+  <si>
+    <t>New York Giants</t>
+  </si>
+  <si>
+    <t>Philadelphia Eagles</t>
+  </si>
+  <si>
+    <t>Washington Commanders</t>
+  </si>
+  <si>
+    <t>Chicago Bears</t>
+  </si>
+  <si>
+    <t>Detroit Lions</t>
+  </si>
+  <si>
+    <t>Green Bay Packers</t>
+  </si>
+  <si>
+    <t>Minnesota Vikings</t>
+  </si>
+  <si>
+    <t>Atlanta Falcons</t>
+  </si>
+  <si>
+    <t>Carolina Panthers</t>
+  </si>
+  <si>
+    <t>New Orleans Saints</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers</t>
+  </si>
+  <si>
+    <t>Arizona Cardinals</t>
+  </si>
+  <si>
+    <t>Los Angeles Rams</t>
+  </si>
+  <si>
+    <t>San Francisco 49ers</t>
+  </si>
+  <si>
+    <t>Seattle Seahawks</t>
+  </si>
+  <si>
+    <t>Indianapolis Colts</t>
+  </si>
+  <si>
+    <t>Tennessee Titans</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,14 +485,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADF1CD2-1FEB-4105-B7FC-B561B248CD13}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>